<commit_message>
Primera versión punto 5 y modificacion excel
</commit_message>
<xml_diff>
--- a/Parte 2/Gastos_e_inversiones_excel.xlsx
+++ b/Parte 2/Gastos_e_inversiones_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maribelms\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maribelms\Desktop\empresa 2\PlanDeEmpresa\Parte 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5D1260-02AF-4F62-A169-1BFF69530222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8A614B-F858-48C3-AFB0-DEDAE7425137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FCBE7B65-FBE3-445A-A1AA-935D45284AA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Concepto</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>https://www.calculat.org/es/energia/consumo-de-electricidad/</t>
+  </si>
+  <si>
+    <t>TOTAL G+I</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +293,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,9 +316,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,6 +326,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -653,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BFD274-08C5-4E45-ADB0-1502128382B8}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="103" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="103" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -667,31 +677,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -1204,39 +1214,39 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E48" s="1">
+      <c r="E48" s="5">
         <f>SUM(E3:E45)</f>
         <v>581098.65999999992</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4" t="s">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1254,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="E53">
-        <f>C53*D53</f>
+        <f t="shared" ref="E53:E64" si="0">C53*D53</f>
         <v>6990</v>
       </c>
     </row>
@@ -1272,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="E54">
-        <f>C54*D54</f>
+        <f t="shared" si="0"/>
         <v>1697</v>
       </c>
     </row>
@@ -1287,11 +1297,11 @@
         <v>64.400000000000006</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E55">
-        <f>C55*D55</f>
-        <v>257.60000000000002</v>
+        <f t="shared" si="0"/>
+        <v>644</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
@@ -1308,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="E56">
-        <f>C56*D56</f>
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
     </row>
@@ -1326,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E57">
-        <f>C57*D57</f>
+        <f t="shared" si="0"/>
         <v>515</v>
       </c>
     </row>
@@ -1334,7 +1344,7 @@
       <c r="A58" t="s">
         <v>49</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C58">
@@ -1344,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="E58">
-        <f>C58*D58</f>
+        <f t="shared" si="0"/>
         <v>1290</v>
       </c>
     </row>
@@ -1362,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="E59">
-        <f>C59*D59</f>
+        <f t="shared" si="0"/>
         <v>1450</v>
       </c>
     </row>
@@ -1377,11 +1387,11 @@
         <v>974.39</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60">
-        <f>C60*D60</f>
-        <v>1948.78</v>
+        <f t="shared" si="0"/>
+        <v>2923.17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
@@ -1398,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="E61">
-        <f>C61*D61</f>
+        <f t="shared" si="0"/>
         <v>2601</v>
       </c>
     </row>
@@ -1413,11 +1423,11 @@
         <v>159</v>
       </c>
       <c r="D62">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E62">
-        <f>C62*D62</f>
-        <v>2385</v>
+        <f t="shared" si="0"/>
+        <v>2862</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
@@ -1431,11 +1441,11 @@
         <v>209</v>
       </c>
       <c r="D63">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E63">
-        <f>C63*D63</f>
-        <v>1254</v>
+        <f t="shared" si="0"/>
+        <v>2090</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
@@ -1452,19 +1462,30 @@
         <v>10</v>
       </c>
       <c r="E64">
-        <f>C64*D64</f>
+        <f t="shared" si="0"/>
         <v>79.900000000000006</v>
       </c>
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E67" s="1">
+      <c r="E67" s="5">
         <f>SUM(E53:E64)</f>
-        <v>20633.280000000002</v>
+        <v>23307.07</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E70" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E71" s="6">
+        <f>SUM(E48,E67)</f>
+        <v>604405.72999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ultimos retoques parte 2
</commit_message>
<xml_diff>
--- a/Parte 2/Gastos_e_inversiones_excel.xlsx
+++ b/Parte 2/Gastos_e_inversiones_excel.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maribelms\Desktop\empresa 2\PlanDeEmpresa\Parte 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Centro d'estudios Edix\Classes\2º Año\Empresa e Iniciativa\Actividades\PlanDeEmpresa\Parte 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8A614B-F858-48C3-AFB0-DEDAE7425137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA87E5A-CF0C-46FA-92B6-BA4D49E464D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FCBE7B65-FBE3-445A-A1AA-935D45284AA7}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{FCBE7B65-FBE3-445A-A1AA-935D45284AA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t>Concepto</t>
   </si>
@@ -251,14 +240,71 @@
     <t>https://www.calculat.org/es/energia/consumo-de-electricidad/</t>
   </si>
   <si>
-    <t>TOTAL G+I</t>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>suponiendo que hacemos 3 proyectos al año(duracion 5meses aprox)</t>
+  </si>
+  <si>
+    <t>Amortizado por año</t>
+  </si>
+  <si>
+    <t>amortización en años</t>
+  </si>
+  <si>
+    <t>TOTAL AMORTIZACIÓN</t>
+  </si>
+  <si>
+    <t>Precio tecnico del producto</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>precio de venta del producto</t>
+  </si>
+  <si>
+    <t>TOTAL G+A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aportacion de los promotores </t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Aportacion programa ICO</t>
+  </si>
+  <si>
+    <t>ICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para el sacar el precio de venta sobre la aportacion del programa ICO ya que nosotros </t>
+  </si>
+  <si>
+    <t>aportamos el 25% asi podemos bajar el precio del producto</t>
+  </si>
+  <si>
+    <t>Calculo del precio de venta</t>
+  </si>
+  <si>
+    <t>Pv</t>
+  </si>
+  <si>
+    <t>le hemos aplicado un 20% de margen</t>
+  </si>
+  <si>
+    <t>Gastos restantes que quedan por cubrir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +324,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,7 +380,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -663,20 +724,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BFD274-08C5-4E45-ADB0-1502128382B8}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="103" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.1328125" customWidth="1"/>
-    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -685,7 +748,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +766,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -718,7 +781,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -733,7 +796,7 @@
         <v>3608.6400000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -748,7 +811,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -763,7 +826,7 @@
         <v>3608.6400000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -778,7 +841,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -793,7 +856,7 @@
         <v>3608.6400000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -808,7 +871,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -824,7 +887,7 @@
         <v>9144</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -839,7 +902,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -855,7 +918,7 @@
         <v>5486.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -870,7 +933,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -886,7 +949,7 @@
         <v>9144</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -901,7 +964,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -917,7 +980,7 @@
         <v>9144</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -932,7 +995,7 @@
         <v>21600</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -948,7 +1011,7 @@
         <v>6583.68</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -963,7 +1026,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -979,7 +1042,7 @@
         <v>5486.4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -997,7 +1060,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1078,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1033,7 +1096,7 @@
         <v>76.800000000000011</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1051,7 +1114,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1132,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1087,25 +1150,25 @@
         <v>444</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C37">
-        <v>6083.33</v>
+      <c r="C37" s="6">
+        <v>608.33000000000004</v>
       </c>
       <c r="D37">
         <v>12</v>
       </c>
       <c r="E37">
         <f>C37*D37</f>
-        <v>72999.959999999992</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+        <v>7299.9600000000009</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1123,7 +1186,7 @@
         <v>220500</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>62</v>
       </c>
@@ -1141,7 +1204,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -1159,7 +1222,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -1177,7 +1240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -1195,7 +1258,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -1213,18 +1276,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E47" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E48" s="5">
         <f>SUM(E3:E45)</f>
-        <v>581098.65999999992</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+        <v>515398.66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3" t="s">
         <v>36</v>
@@ -1232,8 +1295,10 @@
       <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,8 +1314,14 @@
       <c r="E52" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -1267,8 +1338,14 @@
         <f t="shared" ref="E53:E64" si="0">C53*D53</f>
         <v>6990</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" s="7">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -1285,8 +1362,15 @@
         <f t="shared" si="0"/>
         <v>1697</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54" s="7">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <f>E54/F54</f>
+        <v>565.66666666666663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -1303,8 +1387,15 @@
         <f t="shared" si="0"/>
         <v>644</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55" s="7">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <f>E55/F55</f>
+        <v>214.66666666666666</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -1321,8 +1412,15 @@
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" s="7">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <f>E56/F56</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -1339,8 +1437,15 @@
         <f t="shared" si="0"/>
         <v>515</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57" s="7">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <f>E57/F57</f>
+        <v>171.66666666666666</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -1357,8 +1462,15 @@
         <f t="shared" si="0"/>
         <v>1290</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58" s="7">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <f>E58/F58</f>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -1375,8 +1487,15 @@
         <f t="shared" si="0"/>
         <v>1450</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59" s="7">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <f>E59/3</f>
+        <v>483.33333333333331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1393,8 +1512,15 @@
         <f t="shared" si="0"/>
         <v>2923.17</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60" s="7">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <f>E60/3</f>
+        <v>974.39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -1411,8 +1537,15 @@
         <f t="shared" si="0"/>
         <v>2601</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61" s="7">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <f>E61/3</f>
+        <v>867</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -1429,8 +1562,15 @@
         <f t="shared" si="0"/>
         <v>2862</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F62" s="7">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <f>E62/F62</f>
+        <v>954</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -1447,8 +1587,15 @@
         <f t="shared" si="0"/>
         <v>2090</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F63" s="7">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <f>E63/F63</f>
+        <v>696.66666666666663</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -1465,34 +1612,166 @@
         <f t="shared" si="0"/>
         <v>79.900000000000006</v>
       </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="F64" s="7">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <f>E64/F64</f>
+        <v>26.633333333333336</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E66" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="G66" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E67" s="5">
         <f>SUM(E53:E64)</f>
         <v>23307.07</v>
       </c>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="G67" s="5">
+        <f>SUM(G53:G64)</f>
+        <v>7769.0233333333335</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E70" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E71" s="5">
+        <f>SUM(E48,G67)</f>
+        <v>523167.68333333329</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D80" s="8">
+        <f>E71*0.25</f>
+        <v>130791.92083333332</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="8">
+        <f>E71-D80</f>
+        <v>392375.76249999995</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E71" s="6">
-        <f>SUM(E48,E67)</f>
-        <v>604405.72999999986</v>
-      </c>
+      <c r="D88" s="8">
+        <f>D81</f>
+        <v>392375.76249999995</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D89" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>77</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D90" s="8">
+        <f>D88/D89</f>
+        <v>130791.92083333332</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" s="5">
+        <f>D90*(1+0.2)</f>
+        <v>156950.30499999999</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F92" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E92:F92"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B58" r:id="rId1" xr:uid="{376B4F39-FD62-4E65-B3A3-82617D25DF75}"/>
+    <hyperlink ref="B37" r:id="rId2" xr:uid="{07D66F7B-DEBA-4FAE-93DA-6EDFF8B6BFDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>